<commit_message>
Processed Results - updated measures
</commit_message>
<xml_diff>
--- a/Processed Results/Mi 9T/Accelerometer.xlsx
+++ b/Processed Results/Mi 9T/Accelerometer.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luuk1\Downloads\Processed Results\Mi 9T\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luuk1\Desktop\Bachelor Project\BachelorProject\Processed Results\Mi 9T\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA16B85-434A-468D-B329-13E8B9F3C5BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8C25CF-3FA4-4A13-A1CA-2168631FCE1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BD96B59B-3C3E-42C2-91CD-DAE8785DB1E9}"/>
   </bookViews>
@@ -18,8 +18,6 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Blad1!$A$2:$A$31</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Blad1!$B$2:$B$31</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Blad1!$A$2:$A$31</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Blad1!$B$2:$B$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="12">
   <si>
     <t>Mean line</t>
   </si>
@@ -69,6 +67,12 @@
   </si>
   <si>
     <t>Q3</t>
+  </si>
+  <si>
+    <t>Std</t>
+  </si>
+  <si>
+    <t>Relative std</t>
   </si>
 </sst>
 </file>
@@ -2386,7 +2390,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y15" sqref="Y15"/>
+      <selection activeCell="E16" sqref="D15:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2576,6 +2580,12 @@
       <c r="B15" s="1">
         <v>101.79071999999999</v>
       </c>
+      <c r="D15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -2583,6 +2593,14 @@
       </c>
       <c r="B16" s="1">
         <v>101.154528</v>
+      </c>
+      <c r="D16">
+        <f>STDEV(B2:B31)</f>
+        <v>0.89068185803241073</v>
+      </c>
+      <c r="E16">
+        <f>(D16 / E3) *100</f>
+        <v>0.87210580895007472</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>